<commit_message>
adicionei o gráfico de gastos de aparecida
</commit_message>
<xml_diff>
--- a/Dados/Dados de gastos/Aparecida/med-aparecida-compilado.xlsx
+++ b/Dados/Dados de gastos/Aparecida/med-aparecida-compilado.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\API\Dados\Dados de gastos\Aparecida\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Área de Trabalho/API/Dados/Dados de gastos/Aparecida/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_037B71745E941D913A91AF3907D887EEF1E739A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1D4E5B-78F1-40A7-BB0F-3C80376FC3B8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7455"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -44,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
@@ -121,7 +133,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -152,7 +164,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Aplicação</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de recursos na saúde por ano</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -184,7 +225,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15383114610673668"/>
+          <c:y val="0.18132890792604459"/>
+          <c:w val="0.8156132983377079"/>
+          <c:h val="0.60158823463743494"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -194,7 +245,7 @@
           <c:order val="4"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -202,6 +253,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-727E-4B16-92F1-30CC0FAE10D0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-727E-4B16-92F1-30CC0FAE10D0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>Planilha1!$B$1:$D$1</c:f>
@@ -343,7 +432,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$1:$D$1</c15:sqref>
@@ -367,7 +456,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$2:$D$2</c15:sqref>
@@ -389,7 +478,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-8956-406B-AF1A-40528F8E0230}"/>
                   </c:ext>
@@ -412,7 +501,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$1:$D$1</c15:sqref>
@@ -436,7 +525,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$3:$D$3</c15:sqref>
@@ -458,7 +547,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-8956-406B-AF1A-40528F8E0230}"/>
                   </c:ext>
@@ -481,7 +570,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$1:$D$1</c15:sqref>
@@ -505,7 +594,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$B$4:$D$4</c15:sqref>
@@ -527,7 +616,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-8956-406B-AF1A-40528F8E0230}"/>
                   </c:ext>
@@ -544,6 +633,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Ano</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -609,7 +753,75 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Gasto</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> (R$)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.888888888888889E-2"/>
+              <c:y val="0.43701050957240695"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -643,6 +855,71 @@
         <c:crossAx val="53080304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout>
+              <c:manualLayout>
+                <c:xMode val="edge"/>
+                <c:yMode val="edge"/>
+                <c:x val="3.6680664916885389E-2"/>
+                <c:y val="0.19599557613251892"/>
+              </c:manualLayout>
+            </c:layout>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US"/>
+                    <a:t>em Milhões</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1237,19 +1514,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:colOff>473075</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1529,20 +1812,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1839,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1570,7 +1853,7 @@
         <v>4519240.92</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1868,7 @@
         <v>11021418.42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1600,7 +1883,7 @@
         <v>16302742.550000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1900,7 @@
         <v>31843401.890000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>SUM(C2+C3)</f>
         <v>10145547.09</v>

</xml_diff>